<commit_message>
Fix: Configure Config file
- Configured the Config file to not Orchestrator
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joking Genius\Documents\UiPath\Calculate-Client-Security-Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -85,23 +84,12 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -120,12 +108,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
     <t>MaxConsecutiveSystemExceptions</t>
   </si>
   <si>
@@ -159,14 +141,26 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>ACME_Credentials</t>
+  </si>
+  <si>
+    <t>ACME_Credential</t>
+  </si>
+  <si>
+    <t>ACME_URL_Link</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/login</t>
+  </si>
+  <si>
+    <t>Calculate_Client_Security_Hash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +184,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,21 +208,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -534,19 +536,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -583,39 +585,35 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="43.2">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="29">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1606,29 +1604,30 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,26 +1664,26 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1707,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1729,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1740,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1751,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2779,17 +2778,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2800,7 +2799,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Fix: Configured for Tabular Data
- Configured the REFramework to use Tabular Data from an input file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>Calculate_Client_Security_Hash</t>
+  </si>
+  <si>
+    <t>InputFilePath</t>
+  </si>
+  <si>
+    <t>Data\Input\ACME-Transactions.xlsx</t>
+  </si>
+  <si>
+    <t>LoggingFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\Logs.xlsx</t>
   </si>
 </sst>
 </file>
@@ -540,7 +552,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -615,9 +627,23 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Feat: Created ACME_Open xaml
- Implemented logic to open Edge and log in to ACME
- Implemented the Business Exception logic
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,30 @@
   </si>
   <si>
     <t>Data\Output\Logs.xlsx</t>
+  </si>
+  <si>
+    <t>ExceptionEmailAddress</t>
+  </si>
+  <si>
+    <t>exceptions@acme-test.com</t>
+  </si>
+  <si>
+    <t>Login_BE_Subject</t>
+  </si>
+  <si>
+    <t>Login_BE_Body</t>
+  </si>
+  <si>
+    <t>ACME Authentication - Invalid Credentials</t>
+  </si>
+  <si>
+    <t>Hello, 
+The username or the email is incorrect. Please check and restart
+Thank you,
+Calculate Client Security Hash Automation</t>
+  </si>
+  <si>
+    <t>Outlook_Credentials</t>
   </si>
 </sst>
 </file>
@@ -552,7 +576,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -645,9 +669,23 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -1634,9 +1672,10 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1644,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1828,8 +1867,22 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Feat: Configured SHA1 Generator
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Outlook_Credentials</t>
+  </si>
+  <si>
+    <t>SHA1OnlineGeneratorURL</t>
+  </si>
+  <si>
+    <t>https://sha1online.net/</t>
   </si>
 </sst>
 </file>
@@ -575,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" activeCellId="1" sqref="B16 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -687,7 +693,14 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1673,9 +1686,10 @@
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
     <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B16" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Feat: No Data Exception
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joking Genius\Documents\UiPath\Calculate-Client-Security-Hash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\Calculate-Client-Security-Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B4C59A-0928-47C4-8E1A-071D3C5524F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -189,9 +190,6 @@
 Calculate Client Security Hash Automation</t>
   </si>
   <si>
-    <t>Outlook_Credentials</t>
-  </si>
-  <si>
     <t>SHA1OnlineGeneratorURL</t>
   </si>
   <si>
@@ -201,7 +199,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -255,9 +253,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,19 +576,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z996"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -628,7 +626,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="29">
+    <row r="3" spans="1:26" ht="30">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -683,24 +681,19 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B13" s="4"/>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
-        <v>54</v>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1679,14 +1672,12 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
-    <hyperlink ref="B16" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -1694,19 +1685,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1743,7 +1734,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1754,7 +1745,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1868,7 +1859,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -2871,17 +2862,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>